<commit_message>
Fix excel files and conf
</commit_message>
<xml_diff>
--- a/Performer/Data/Config.xlsx
+++ b/Performer/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -182,16 +182,13 @@
     <t>GmailPort</t>
   </si>
   <si>
-    <t>MonthReportsFolderPath</t>
-  </si>
-  <si>
     <t>ReportsPath</t>
   </si>
   <si>
-    <t>ResultExcelFilePath</t>
-  </si>
-  <si>
     <t>SiteUploadPath</t>
+  </si>
+  <si>
+    <t>TempFolderPath</t>
   </si>
 </sst>
 </file>
@@ -2831,7 +2828,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2916,10 +2913,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -2927,10 +2924,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -2938,26 +2935,16 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>